<commit_message>
1. Rename 2. 添加BFS, DFS, TopologicalSort, SCC相关算法代码
</commit_message>
<xml_diff>
--- a/Algorithms/Summary.xlsx
+++ b/Algorithms/Summary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>MajorityElement</t>
   </si>
@@ -86,6 +86,10 @@
   </si>
   <si>
     <t>低级bug</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FindKthLargest</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -511,10 +515,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -565,6 +569,11 @@
         <v>18</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
1. 添加FindKthLargest and SortArrayByParityII算法代码 2. 更新Sumarry.xlsx统计
</commit_message>
<xml_diff>
--- a/Algorithms/Summary.xlsx
+++ b/Algorithms/Summary.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Devide&amp;Conquer" sheetId="1" r:id="rId1"/>
     <sheet name="Heap" sheetId="2" r:id="rId2"/>
+    <sheet name="Sort" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>MajorityElement</t>
   </si>
@@ -68,28 +69,86 @@
     <t>KClosest</t>
   </si>
   <si>
+    <t>FrequencySort</t>
+  </si>
+  <si>
+    <t>第一次性能不够好, 改为StringBuilder就好了，不是核心问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TopKFrequent</t>
+  </si>
+  <si>
+    <t>KthSmallest</t>
+  </si>
+  <si>
+    <t>低级bug</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FindKthLargest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>思考比较透彻</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FrequencySort</t>
-  </si>
-  <si>
-    <t>第一次性能不够好, 改为StringBuilder就好了，不是核心问题</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TopKFrequent</t>
-  </si>
-  <si>
-    <t>KthSmallest</t>
-  </si>
-  <si>
-    <t>低级bug</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FindKthLargest</t>
+    <t>思考比较透彻</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SortArrayByParityII</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一遍过，可能还有更好的解法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RelativeSortArray</t>
+  </si>
+  <si>
+    <t>慢</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字符串交错的算法不熟悉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NthSuperUglyNumber</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsPossible</t>
+  </si>
+  <si>
+    <t>RearrangeBarcodes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReorganizeString</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>和ReorganizeString基本一样</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NthUglyNumber</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>错误较多，多次才解决</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>错误较多，多次才解决</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>如何组织heap想的不透彻</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -97,7 +156,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,8 +177,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -150,6 +216,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -163,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -171,6 +243,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -457,13 +531,13 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="19.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -471,13 +545,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -485,7 +559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -493,7 +567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -501,7 +575,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -515,24 +589,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -540,38 +614,81 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="B6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="6" t="s">
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>19</v>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -579,4 +696,40 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>